<commit_message>
change data return more detail when import
</commit_message>
<xml_diff>
--- a/Metadata.API/ReportTemplates/BangTongHopChiPhiBT.xlsx
+++ b/Metadata.API/ReportTemplates/BangTongHopChiPhiBT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\GPMB\Flutter\KiemKeGPMB\KiemKeGPMB\baocaoGPMB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE DO AN\13-11\YOLO\Metadata.API\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E18CF4C-6516-4B8C-90F8-DE8E6C81CEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BangTongHopChiPhi" sheetId="1" r:id="rId1"/>
@@ -158,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,6 +251,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -261,9 +265,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,11 +545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9:Q10"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,26 +573,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="K1" s="15" t="s">
+      <c r="C1" s="15"/>
+      <c r="K1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="K2" s="15" t="s">
+      <c r="C2" s="16"/>
+      <c r="K2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
@@ -615,57 +616,57 @@
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17" t="s">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="17" t="s">
+      <c r="N9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="17" t="s">
+      <c r="O9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="17" t="s">
+      <c r="P9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="17" t="s">
+      <c r="Q9" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="8" t="s">
         <v>5</v>
       </c>
@@ -678,15 +679,15 @@
       <c r="H10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
     </row>
     <row r="11" spans="1:17" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -742,12 +743,12 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -801,15 +802,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -820,6 +812,15 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>